<commit_message>
Update structural design script configuration and regenerate outputs
- Update `structural_design.py` CONFIG: Change FLOORS from 5 to 3.
- Regenerate `My Drawing_FINAL_V2.dxf` and `My Drawing_DATA_V2.xlsx` with new configuration.
</commit_message>
<xml_diff>
--- a/My Drawing_DATA_V2.xlsx
+++ b/My Drawing_DATA_V2.xlsx
@@ -2177,11 +2177,11 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1714</v>
+        <v>1028</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2.5x2.5x0.6</t>
+          <t>2.0x2.0x0.6</t>
         </is>
       </c>
     </row>
@@ -2197,11 +2197,11 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1714</v>
+        <v>1028</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2.5x2.5x0.6</t>
+          <t>2.0x2.0x0.6</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1714</v>
+        <v>1028</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -2237,7 +2237,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1714</v>
+        <v>1028</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -2257,7 +2257,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1714</v>
+        <v>1028</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -2277,7 +2277,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1714</v>
+        <v>1028</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -2297,7 +2297,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1714</v>
+        <v>1028</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1714</v>
+        <v>1028</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -2337,11 +2337,11 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1714</v>
+        <v>1028</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.5x2.5x0.6</t>
+          <t>2.0x2.0x0.6</t>
         </is>
       </c>
     </row>
@@ -2357,11 +2357,11 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1714</v>
+        <v>1028</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2.5x2.5x0.6</t>
+          <t>2.0x2.0x0.6</t>
         </is>
       </c>
     </row>
@@ -2377,11 +2377,11 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1714</v>
+        <v>1028</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2.5x2.5x0.6</t>
+          <t>2.0x2.0x0.6</t>
         </is>
       </c>
     </row>
@@ -2397,11 +2397,11 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2.3x2.3x0.6</t>
+          <t>1.8x1.8x0.6</t>
         </is>
       </c>
     </row>
@@ -2417,7 +2417,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -2437,7 +2437,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -2457,7 +2457,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -2477,7 +2477,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -2497,7 +2497,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -2517,7 +2517,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -2537,7 +2537,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -2557,7 +2557,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -2577,11 +2577,11 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2.3x2.3x0.6</t>
+          <t>1.8x1.8x0.6</t>
         </is>
       </c>
     </row>
@@ -2597,11 +2597,11 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2.3x2.3x0.6</t>
+          <t>1.8x1.8x0.6</t>
         </is>
       </c>
     </row>
@@ -2617,11 +2617,11 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2.3x2.3x0.6</t>
+          <t>1.8x1.8x0.6</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1428</v>
+        <v>857</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>

</xml_diff>